<commit_message>
Mon Jan 26 15:43:15 MST 2015
</commit_message>
<xml_diff>
--- a/Correlations_ICBP_Single_Multi .xlsx
+++ b/Correlations_ICBP_Single_Multi .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="340" windowWidth="24880" windowHeight="13460" tabRatio="500"/>
+    <workbookView xWindow="1080" yWindow="340" windowWidth="37680" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Correlations_ICBP_Single_Multi " sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="223">
   <si>
     <t>X17.AAG</t>
   </si>
@@ -291,9 +291,6 @@
     <t>ZM447439</t>
   </si>
   <si>
-    <t>akt_s_a</t>
-  </si>
-  <si>
     <t>bad_s_a</t>
   </si>
   <si>
@@ -343,9 +340,6 @@
   </si>
   <si>
     <t xml:space="preserve">all_4   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi Pathway </t>
   </si>
   <si>
     <t>Notes:</t>
@@ -683,13 +677,56 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Anthelmintic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHFR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DNA synthesis/ repair</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDK1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mitotic kinesin KSP (Eg5) inhibitor</t>
+  </si>
+  <si>
+    <t>topoisomerase </t>
+  </si>
+  <si>
+    <t>IGFR</t>
+  </si>
+  <si>
+    <t>HDAC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Microtubule</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AURKA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>akt_single_adaptive</t>
+  </si>
+  <si>
+    <t>Multi Pathway Adaptive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -745,8 +782,14 @@
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF545454"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,6 +838,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -805,7 +854,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -817,8 +866,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -852,18 +905,29 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1195,11 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CN231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane xSplit="15440" ySplit="2920" topLeftCell="CA16" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="BW2" sqref="BW2"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
-      <selection pane="bottomRight" activeCell="CC25" sqref="CC25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1208,494 +1269,554 @@
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92">
-      <c r="A1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:92" s="23" customFormat="1">
+      <c r="A1" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AO1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AV1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AX1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AY1" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="AZ1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BA1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BB1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BC1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BD1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BE1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BF1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BG1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BH1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BI1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BJ1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BK1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BL1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BM1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BN1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BO1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BP1" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BQ1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BR1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BS1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BT1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BU1" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BV1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BW1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BX1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BY1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="BZ1" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CA1" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CB1" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CC1" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CD1" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CE1" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CF1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CG1" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CH1" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CI1" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CJ1" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CK1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CL1" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CM1" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CN1" s="23" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:92" ht="45">
       <c r="A2" s="1"/>
       <c r="C2" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>133</v>
+      <c r="G2" t="s">
+        <v>113</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I2" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE2" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK2" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL2" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM2" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AN2" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="AS2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU2" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="AV2" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AW2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="AX2" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY2" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AZ2" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="BA2" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BB2" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BC2" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="BD2" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="BE2" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="BF2" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH2" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="BI2" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="BJ2" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="BL2" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="BM2" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="BN2" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="BO2" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="BP2" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="BQ2" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="BR2" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="BS2" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="BU2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>114</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="BX2" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="BY2" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="BZ2" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="CA2" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="CB2" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="AA2" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="AE2" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="AI2" s="12" t="s">
+      <c r="CC2" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="CD2" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="CE2" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="CF2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="CG2" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>217</v>
+      </c>
+      <c r="CI2" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="CJ2" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="AJ2" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL2" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="AM2" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN2" s="7" t="s">
+      <c r="CK2" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="CL2" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="CM2" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="AO2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP2" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="AQ2" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="AR2" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="AS2" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AT2" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="AU2" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="AV2" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="AX2" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="AY2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="AZ2" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="BA2" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="BB2" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="BE2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="BF2" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="BG2" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="BH2" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="BI2" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="BJ2" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="BK2" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="BM2" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="BN2" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="BP2" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="BQ2" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="BU2" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="BW2" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="BY2" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="BZ2" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="CA2" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="CB2" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="CC2" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="CE2" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="CF2" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="CI2" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="CK2" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="CM2" s="7" t="s">
-        <v>186</v>
+      <c r="CN2" s="7" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:92" s="3" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="3">
         <v>5.6771098872287401E-2</v>
@@ -1904,7 +2025,7 @@
       <c r="BS3" s="3">
         <v>-0.14794500988383999</v>
       </c>
-      <c r="BT3" s="3">
+      <c r="BT3" s="20">
         <v>0.33233999297278699</v>
       </c>
       <c r="BU3" s="14">
@@ -1943,7 +2064,7 @@
       <c r="CF3" s="14">
         <v>0.32669950729449299</v>
       </c>
-      <c r="CG3" s="3">
+      <c r="CG3" s="20">
         <v>0.56092422744007098</v>
       </c>
       <c r="CH3" s="4">
@@ -1952,10 +2073,10 @@
       <c r="CI3" s="3">
         <v>-0.30306340064230503</v>
       </c>
-      <c r="CJ3" s="3">
+      <c r="CJ3" s="20">
         <v>0.63394183369596102</v>
       </c>
-      <c r="CK3" s="3">
+      <c r="CK3" s="20">
         <v>0.227814528507507</v>
       </c>
       <c r="CL3" s="3">
@@ -1970,10 +2091,10 @@
     </row>
     <row r="4" spans="1:92" s="3" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="3">
         <v>8.0241837556156603E-2</v>
@@ -2182,7 +2303,7 @@
       <c r="BS4" s="3">
         <v>-5.6957618201357002E-2</v>
       </c>
-      <c r="BT4" s="3">
+      <c r="BT4" s="20">
         <v>0.27138030783806399</v>
       </c>
       <c r="BU4" s="14">
@@ -2221,7 +2342,7 @@
       <c r="CF4" s="14">
         <v>0.322596257820146</v>
       </c>
-      <c r="CG4" s="3">
+      <c r="CG4" s="20">
         <v>0.472918173993983</v>
       </c>
       <c r="CH4" s="4">
@@ -2230,10 +2351,10 @@
       <c r="CI4" s="3">
         <v>-0.174539044621454</v>
       </c>
-      <c r="CJ4" s="3">
+      <c r="CJ4" s="20">
         <v>0.51885155796617599</v>
       </c>
-      <c r="CK4" s="3">
+      <c r="CK4" s="20">
         <v>0.29901146558230901</v>
       </c>
       <c r="CL4" s="3">
@@ -2248,10 +2369,10 @@
     </row>
     <row r="5" spans="1:92" s="3" customFormat="1">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="3">
         <v>0.15253380742842701</v>
@@ -2460,7 +2581,7 @@
       <c r="BS5" s="3">
         <v>-0.102816048828268</v>
       </c>
-      <c r="BT5" s="3">
+      <c r="BT5" s="20">
         <v>0.32366884421251302</v>
       </c>
       <c r="BU5" s="14">
@@ -2499,7 +2620,7 @@
       <c r="CF5" s="14">
         <v>0.307970229967303</v>
       </c>
-      <c r="CG5" s="3">
+      <c r="CG5" s="20">
         <v>0.47233464218323101</v>
       </c>
       <c r="CH5" s="4">
@@ -2508,10 +2629,10 @@
       <c r="CI5" s="3">
         <v>-0.248098899869309</v>
       </c>
-      <c r="CJ5" s="3">
+      <c r="CJ5" s="20">
         <v>0.57491494697330803</v>
       </c>
-      <c r="CK5" s="3">
+      <c r="CK5" s="20">
         <v>0.26899415277343303</v>
       </c>
       <c r="CL5" s="3">
@@ -2526,10 +2647,10 @@
     </row>
     <row r="6" spans="1:92" s="3" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3">
         <v>0.18966366354544201</v>
@@ -2738,7 +2859,7 @@
       <c r="BS6" s="3">
         <v>-0.18242308674691901</v>
       </c>
-      <c r="BT6" s="3">
+      <c r="BT6" s="20">
         <v>0.181092482301108</v>
       </c>
       <c r="BU6" s="14">
@@ -2777,7 +2898,7 @@
       <c r="CF6" s="14">
         <v>0.28500822550955202</v>
       </c>
-      <c r="CG6" s="3">
+      <c r="CG6" s="20">
         <v>0.57070890326202495</v>
       </c>
       <c r="CH6" s="4">
@@ -2786,10 +2907,10 @@
       <c r="CI6" s="3">
         <v>-0.12810201759539599</v>
       </c>
-      <c r="CJ6" s="3">
+      <c r="CJ6" s="20">
         <v>0.59792486337422601</v>
       </c>
-      <c r="CK6" s="3">
+      <c r="CK6" s="20">
         <v>0.44692708956791</v>
       </c>
       <c r="CL6" s="3">
@@ -2804,10 +2925,10 @@
     </row>
     <row r="7" spans="1:92" s="3" customFormat="1">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="3">
         <v>5.1340559177278498E-2</v>
@@ -3016,7 +3137,7 @@
       <c r="BS7" s="3">
         <v>-0.24068996843529999</v>
       </c>
-      <c r="BT7" s="3">
+      <c r="BT7" s="20">
         <v>0.125334771974906</v>
       </c>
       <c r="BU7" s="14">
@@ -3055,7 +3176,7 @@
       <c r="CF7" s="14">
         <v>0.31986307859332802</v>
       </c>
-      <c r="CG7" s="3">
+      <c r="CG7" s="20">
         <v>0.647121169301767</v>
       </c>
       <c r="CH7" s="4">
@@ -3064,10 +3185,10 @@
       <c r="CI7" s="3">
         <v>-0.151254727660389</v>
       </c>
-      <c r="CJ7" s="3">
+      <c r="CJ7" s="20">
         <v>0.60292203456528304</v>
       </c>
-      <c r="CK7" s="3">
+      <c r="CK7" s="20">
         <v>0.45361204696558799</v>
       </c>
       <c r="CL7" s="3">
@@ -3082,10 +3203,10 @@
     </row>
     <row r="8" spans="1:92" s="3" customFormat="1">
       <c r="A8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3">
         <v>0.19371912796142601</v>
@@ -3294,7 +3415,7 @@
       <c r="BS8" s="3">
         <v>2.14734267814757E-2</v>
       </c>
-      <c r="BT8" s="3">
+      <c r="BT8" s="20">
         <v>0.24777491608545499</v>
       </c>
       <c r="BU8" s="14">
@@ -3333,7 +3454,7 @@
       <c r="CF8" s="14">
         <v>0.28460935101482498</v>
       </c>
-      <c r="CG8" s="3">
+      <c r="CG8" s="20">
         <v>0.33403564711939998</v>
       </c>
       <c r="CH8" s="4">
@@ -3342,10 +3463,10 @@
       <c r="CI8" s="3">
         <v>-9.5831999171837795E-2</v>
       </c>
-      <c r="CJ8" s="3">
+      <c r="CJ8" s="20">
         <v>0.39256157097428301</v>
       </c>
-      <c r="CK8" s="3">
+      <c r="CK8" s="20">
         <v>0.32814891104003802</v>
       </c>
       <c r="CL8" s="3">
@@ -3360,10 +3481,10 @@
     </row>
     <row r="9" spans="1:92" s="17" customFormat="1">
       <c r="A9" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>90</v>
+        <v>221</v>
       </c>
       <c r="C9" s="17">
         <v>0.121458488407913</v>
@@ -3620,7 +3741,7 @@
       <c r="CI9" s="17">
         <v>-0.162543888920196</v>
       </c>
-      <c r="CJ9" s="17">
+      <c r="CJ9" s="20">
         <v>0.70837225595019204</v>
       </c>
       <c r="CK9" s="17">
@@ -3638,10 +3759,10 @@
     </row>
     <row r="10" spans="1:92">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>1.80389860675511E-2</v>
@@ -3880,7 +4001,7 @@
       <c r="CC10">
         <v>2.15324788943458E-2</v>
       </c>
-      <c r="CD10">
+      <c r="CD10" s="20">
         <v>0.48416806756612402</v>
       </c>
       <c r="CE10">
@@ -3916,10 +4037,10 @@
     </row>
     <row r="11" spans="1:92">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11">
         <v>-1.9049031449561799E-2</v>
@@ -4158,7 +4279,7 @@
       <c r="CC11">
         <v>6.1715990259296999E-2</v>
       </c>
-      <c r="CD11">
+      <c r="CD11" s="20">
         <v>0.21220742710180701</v>
       </c>
       <c r="CE11">
@@ -4194,10 +4315,10 @@
     </row>
     <row r="12" spans="1:92">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12">
         <v>8.5113080356041995E-2</v>
@@ -4436,7 +4557,7 @@
       <c r="CC12">
         <v>-0.1537277668041</v>
       </c>
-      <c r="CD12">
+      <c r="CD12" s="20">
         <v>0.56231740208843595</v>
       </c>
       <c r="CE12">
@@ -4472,10 +4593,10 @@
     </row>
     <row r="13" spans="1:92">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13">
         <v>0.18098522955480401</v>
@@ -4714,7 +4835,7 @@
       <c r="CC13">
         <v>-8.2998914724056502E-2</v>
       </c>
-      <c r="CD13">
+      <c r="CD13" s="20">
         <v>0.56693821813714196</v>
       </c>
       <c r="CE13">
@@ -4750,10 +4871,10 @@
     </row>
     <row r="14" spans="1:92">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14">
         <v>0.18777238282668901</v>
@@ -4992,7 +5113,7 @@
       <c r="CC14">
         <v>2.14025370938009E-2</v>
       </c>
-      <c r="CD14">
+      <c r="CD14" s="20">
         <v>0.58236717081592404</v>
       </c>
       <c r="CE14">
@@ -5028,10 +5149,10 @@
     </row>
     <row r="15" spans="1:92">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15">
         <v>0.171367542584243</v>
@@ -5270,7 +5391,7 @@
       <c r="CC15">
         <v>-3.2701313519606499E-2</v>
       </c>
-      <c r="CD15">
+      <c r="CD15" s="20">
         <v>0.45837734590127799</v>
       </c>
       <c r="CE15">
@@ -5306,10 +5427,10 @@
     </row>
     <row r="16" spans="1:92">
       <c r="A16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16">
         <v>4.6464131631735101E-2</v>
@@ -5548,7 +5669,7 @@
       <c r="CC16">
         <v>-8.7969006084487794E-2</v>
       </c>
-      <c r="CD16">
+      <c r="CD16" s="20">
         <v>0.34135714516890497</v>
       </c>
       <c r="CE16">
@@ -5584,10 +5705,10 @@
     </row>
     <row r="17" spans="1:92" s="17" customFormat="1">
       <c r="A17" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="17">
         <v>0.20661562625301999</v>
@@ -5862,10 +5983,10 @@
     </row>
     <row r="18" spans="1:92" s="3" customFormat="1">
       <c r="A18" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="3">
         <v>0.104979293789979</v>
@@ -6071,7 +6192,7 @@
       <c r="BR18" s="3">
         <v>-0.197299145746099</v>
       </c>
-      <c r="BS18" s="3">
+      <c r="BS18" s="20">
         <v>0.44769515237406399</v>
       </c>
       <c r="BT18" s="3">
@@ -6104,7 +6225,7 @@
       <c r="CC18" s="3">
         <v>-0.21347729708329599</v>
       </c>
-      <c r="CD18" s="3">
+      <c r="CD18" s="20">
         <v>0.52070498353543704</v>
       </c>
       <c r="CE18" s="3">
@@ -6125,7 +6246,7 @@
       <c r="CJ18" s="3">
         <v>-0.56809183144784503</v>
       </c>
-      <c r="CK18" s="3">
+      <c r="CK18" s="20">
         <v>0.23510505609399299</v>
       </c>
       <c r="CL18" s="3">
@@ -6140,10 +6261,10 @@
     </row>
     <row r="19" spans="1:92" s="3" customFormat="1">
       <c r="A19" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="3">
         <v>3.0632699911760299E-2</v>
@@ -6349,7 +6470,7 @@
       <c r="BR19" s="3">
         <v>-0.111689727304063</v>
       </c>
-      <c r="BS19" s="3">
+      <c r="BS19" s="20">
         <v>0.14514600794189</v>
       </c>
       <c r="BT19" s="3">
@@ -6382,7 +6503,7 @@
       <c r="CC19" s="3">
         <v>-2.1900098847775801E-2</v>
       </c>
-      <c r="CD19" s="3">
+      <c r="CD19" s="20">
         <v>0.56313701165206498</v>
       </c>
       <c r="CE19" s="3">
@@ -6403,7 +6524,7 @@
       <c r="CJ19" s="3">
         <v>-0.61935423015582003</v>
       </c>
-      <c r="CK19" s="3">
+      <c r="CK19" s="20">
         <v>0.33644183794634103</v>
       </c>
       <c r="CL19" s="3">
@@ -6418,10 +6539,10 @@
     </row>
     <row r="20" spans="1:92" s="3" customFormat="1">
       <c r="A20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="3">
         <v>-0.25011763558975297</v>
@@ -6627,7 +6748,7 @@
       <c r="BR20" s="3">
         <v>0.22436528343176099</v>
       </c>
-      <c r="BS20" s="3">
+      <c r="BS20" s="20">
         <v>-0.30793457483196301</v>
       </c>
       <c r="BT20" s="3">
@@ -6660,7 +6781,7 @@
       <c r="CC20" s="3">
         <v>0.26130382236326299</v>
       </c>
-      <c r="CD20" s="3">
+      <c r="CD20" s="20">
         <v>-0.47473760341556798</v>
       </c>
       <c r="CE20" s="3">
@@ -6681,7 +6802,7 @@
       <c r="CJ20" s="3">
         <v>0.50603442068397197</v>
       </c>
-      <c r="CK20" s="3">
+      <c r="CK20" s="20">
         <v>0.21428144730274701</v>
       </c>
       <c r="CL20" s="3">
@@ -6696,10 +6817,10 @@
     </row>
     <row r="21" spans="1:92" s="3" customFormat="1">
       <c r="A21" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" s="3">
         <v>-0.16052699815451399</v>
@@ -6905,7 +7026,7 @@
       <c r="BR21" s="3">
         <v>0.28278648721585697</v>
       </c>
-      <c r="BS21" s="3">
+      <c r="BS21" s="20">
         <v>-0.23026798323057099</v>
       </c>
       <c r="BT21" s="3">
@@ -6938,7 +7059,7 @@
       <c r="CC21" s="3">
         <v>-3.5129965873111603E-2</v>
       </c>
-      <c r="CD21" s="3">
+      <c r="CD21" s="20">
         <v>-0.43491505086222298</v>
       </c>
       <c r="CE21" s="3">
@@ -6959,7 +7080,7 @@
       <c r="CJ21" s="3">
         <v>0.41877756372429598</v>
       </c>
-      <c r="CK21" s="3">
+      <c r="CK21" s="20">
         <v>0.143747285230372</v>
       </c>
       <c r="CL21" s="3">
@@ -6974,10 +7095,10 @@
     </row>
     <row r="22" spans="1:92" s="3" customFormat="1">
       <c r="A22" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="3">
         <v>2.940075703667E-3</v>
@@ -7183,7 +7304,7 @@
       <c r="BR22" s="3">
         <v>6.26819446029586E-3</v>
       </c>
-      <c r="BS22" s="3">
+      <c r="BS22" s="20">
         <v>0.43669768658980901</v>
       </c>
       <c r="BT22" s="3">
@@ -7216,7 +7337,7 @@
       <c r="CC22" s="3">
         <v>-0.28606599746059902</v>
       </c>
-      <c r="CD22" s="3">
+      <c r="CD22" s="20">
         <v>0.25187286099432699</v>
       </c>
       <c r="CE22" s="3">
@@ -7237,7 +7358,7 @@
       <c r="CJ22" s="3">
         <v>-0.29280224137466798</v>
       </c>
-      <c r="CK22" s="3">
+      <c r="CK22" s="20">
         <v>0.14528638362499499</v>
       </c>
       <c r="CL22" s="3">
@@ -7252,10 +7373,10 @@
     </row>
     <row r="23" spans="1:92" s="3" customFormat="1">
       <c r="A23" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" s="3">
         <v>0.13026813990914601</v>
@@ -7461,7 +7582,7 @@
       <c r="BR23" s="3">
         <v>-0.17064899190548699</v>
       </c>
-      <c r="BS23" s="3">
+      <c r="BS23" s="20">
         <v>0.42485399447938099</v>
       </c>
       <c r="BT23" s="3">
@@ -7494,7 +7615,7 @@
       <c r="CC23" s="3">
         <v>-0.26263449633351399</v>
       </c>
-      <c r="CD23" s="3">
+      <c r="CD23" s="20">
         <v>0.492384584072665</v>
       </c>
       <c r="CE23" s="3">
@@ -7515,7 +7636,7 @@
       <c r="CJ23" s="3">
         <v>-0.54789229800474804</v>
       </c>
-      <c r="CK23" s="3">
+      <c r="CK23" s="20">
         <v>0.197232895903656</v>
       </c>
       <c r="CL23" s="3">
@@ -7530,10 +7651,10 @@
     </row>
     <row r="24" spans="1:92" s="17" customFormat="1">
       <c r="A24" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="17">
         <v>-0.215248693940537</v>
@@ -7808,10 +7929,10 @@
     </row>
     <row r="25" spans="1:92">
       <c r="A25" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25">
         <v>-0.27586956076636898</v>
@@ -8059,7 +8180,7 @@
       <c r="CF25" s="14">
         <v>0.27315423698802699</v>
       </c>
-      <c r="CG25">
+      <c r="CG25" s="20">
         <v>0.40024580278648603</v>
       </c>
       <c r="CH25">
@@ -8068,7 +8189,7 @@
       <c r="CI25">
         <v>-0.33575123847569399</v>
       </c>
-      <c r="CJ25">
+      <c r="CJ25" s="20">
         <v>0.34856876012434101</v>
       </c>
       <c r="CK25">
@@ -8086,10 +8207,10 @@
     </row>
     <row r="26" spans="1:92">
       <c r="A26" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26">
         <v>-0.30290668800617998</v>
@@ -8337,7 +8458,7 @@
       <c r="CF26" s="14">
         <v>0.22155310415770399</v>
       </c>
-      <c r="CG26">
+      <c r="CG26" s="20">
         <v>0.35668173226535399</v>
       </c>
       <c r="CH26">
@@ -8346,7 +8467,7 @@
       <c r="CI26">
         <v>-0.30729187880118303</v>
       </c>
-      <c r="CJ26">
+      <c r="CJ26" s="20">
         <v>0.27766973226434299</v>
       </c>
       <c r="CK26">
@@ -8364,10 +8485,10 @@
     </row>
     <row r="27" spans="1:92">
       <c r="A27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27">
         <v>-0.297335727025208</v>
@@ -8615,7 +8736,7 @@
       <c r="CF27" s="14">
         <v>0.220865907272141</v>
       </c>
-      <c r="CG27">
+      <c r="CG27" s="20">
         <v>0.33331205054348501</v>
       </c>
       <c r="CH27">
@@ -8624,7 +8745,7 @@
       <c r="CI27">
         <v>-0.301989311259525</v>
       </c>
-      <c r="CJ27">
+      <c r="CJ27" s="20">
         <v>0.30045602709056302</v>
       </c>
       <c r="CK27">
@@ -8642,10 +8763,10 @@
     </row>
     <row r="28" spans="1:92">
       <c r="A28" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28">
         <v>-0.29833928009092697</v>
@@ -8893,7 +9014,7 @@
       <c r="CF28" s="14">
         <v>0.21755001942608801</v>
       </c>
-      <c r="CG28">
+      <c r="CG28" s="20">
         <v>0.31820524727696903</v>
       </c>
       <c r="CH28">
@@ -8902,7 +9023,7 @@
       <c r="CI28">
         <v>-0.28957907328331101</v>
       </c>
-      <c r="CJ28">
+      <c r="CJ28" s="20">
         <v>0.23603711954793</v>
       </c>
       <c r="CK28">
@@ -8920,10 +9041,10 @@
     </row>
     <row r="29" spans="1:92">
       <c r="A29" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29">
         <v>-0.31761445517757098</v>
@@ -9166,12 +9287,12 @@
         <v>-0.57164881390807298</v>
       </c>
       <c r="CE29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="CF29" s="14">
         <v>0.29021089582258403</v>
       </c>
-      <c r="CG29">
+      <c r="CG29" s="20">
         <v>0.35414151676816502</v>
       </c>
       <c r="CH29">
@@ -9180,7 +9301,7 @@
       <c r="CI29">
         <v>-0.37111700960750599</v>
       </c>
-      <c r="CJ29">
+      <c r="CJ29" s="20">
         <v>0.34732900971339897</v>
       </c>
       <c r="CK29">
@@ -9198,10 +9319,10 @@
     </row>
     <row r="30" spans="1:92">
       <c r="A30" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30">
         <v>-0.302031482393322</v>
@@ -9449,7 +9570,7 @@
       <c r="CF30" s="14">
         <v>0.235645887361665</v>
       </c>
-      <c r="CG30">
+      <c r="CG30" s="20">
         <v>0.39839244931518197</v>
       </c>
       <c r="CH30">
@@ -9458,7 +9579,7 @@
       <c r="CI30">
         <v>-0.32186759191763398</v>
       </c>
-      <c r="CJ30">
+      <c r="CJ30" s="20">
         <v>0.36227402604912101</v>
       </c>
       <c r="CK30">
@@ -9476,10 +9597,10 @@
     </row>
     <row r="31" spans="1:92" s="17" customFormat="1">
       <c r="A31" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="17">
         <v>-0.22101187960160601</v>
@@ -9727,7 +9848,7 @@
       <c r="CF31" s="17">
         <v>-5.1875270692707198E-2</v>
       </c>
-      <c r="CG31" s="17">
+      <c r="CG31" s="20">
         <v>0.25665098383181401</v>
       </c>
       <c r="CH31" s="17">
@@ -9754,44 +9875,44 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B45" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B49" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="110" spans="2:2">
@@ -9802,267 +9923,267 @@
     </row>
     <row r="112" spans="2:2">
       <c r="B112" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="2:2">
       <c r="B113" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="2:2">
       <c r="B114" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="116" spans="2:2">
       <c r="B116" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="2:2">
       <c r="B117" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="2:2">
       <c r="B118" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="2:2">
       <c r="B119" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="2:2">
       <c r="B120" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="2:2">
       <c r="B121" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="2:2">
       <c r="B123" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="125" spans="2:2">
       <c r="B125" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="2:2">
       <c r="B126" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="128" spans="2:2">
       <c r="B128" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="129" spans="2:2">
       <c r="B129" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="130" spans="2:2">
       <c r="B130" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="131" spans="2:2">
       <c r="B131" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="132" spans="2:2">
       <c r="B132" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="133" spans="2:2">
       <c r="B133" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="135" spans="2:2">
       <c r="B135" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="2:2">
       <c r="B138" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="2:2">
       <c r="B140" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="141" spans="2:2">
       <c r="B141" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="142" spans="2:2">
       <c r="B142" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="143" spans="2:2">
       <c r="B143" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="144" spans="2:2">
       <c r="B144" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="145" spans="2:2">
       <c r="B145" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="147" spans="2:2">
       <c r="B147" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="149" spans="2:2">
       <c r="B149" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="156" spans="2:2">
       <c r="B156" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="157" spans="2:2">
       <c r="B157" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="158" spans="2:2">
       <c r="B158" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="159" spans="2:2">
       <c r="B159" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="160" spans="2:2">
       <c r="B160" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="161" spans="2:2">
       <c r="B161" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="163" spans="2:2">
       <c r="B163" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="164" spans="2:2">
       <c r="B164" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="165" spans="2:2">
@@ -10073,197 +10194,197 @@
     </row>
     <row r="167" spans="2:2">
       <c r="B167" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="169" spans="2:2">
       <c r="B169" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="170" spans="2:2">
       <c r="B170" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="173" spans="2:2">
       <c r="B173" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="174" spans="2:2">
       <c r="B174" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="175" spans="2:2">
       <c r="B175" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="176" spans="2:2">
       <c r="B176" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="177" spans="2:2">
       <c r="B177" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="178" spans="2:2">
       <c r="B178" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="179" spans="2:2">
       <c r="B179" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="180" spans="2:2">
       <c r="B180" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="181" spans="2:2">
       <c r="B181" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="182" spans="2:2">
       <c r="B182" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="183" spans="2:2">
       <c r="B183" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="184" spans="2:2">
       <c r="B184" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="185" spans="2:2">
       <c r="B185" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="186" spans="2:2">
       <c r="B186" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="187" spans="2:2">
       <c r="B187" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="188" spans="2:2">
       <c r="B188" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="189" spans="2:2">
       <c r="B189" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="190" spans="2:2">
       <c r="B190" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="191" spans="2:2">
       <c r="B191" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="192" spans="2:2">
       <c r="B192" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="193" spans="2:2">
       <c r="B193" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="194" spans="2:2">
       <c r="B194" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="197" spans="2:2">
       <c r="B197" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="198" spans="2:2">
       <c r="B198" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="199" spans="2:2">
       <c r="B199" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="200" spans="2:2">
       <c r="B200" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="201" spans="2:2">
       <c r="B201" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="202" spans="2:2">
       <c r="B202" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="203" spans="2:2">
       <c r="B203" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="204" spans="2:2">
       <c r="B204" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="205" spans="2:2">
       <c r="B205" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="206" spans="2:2">

</xml_diff>